<commit_message>
Samiksha Mendhe: Task1 is completed for excel
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\da18\Excel\day3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\da18\github data\da18ExcelTask1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF1B623-0182-4CCB-9480-D0A628622328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1317A72E-46D6-461B-9AD3-F95EFC3A0A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -189,10 +189,10 @@
     <t>access</t>
   </si>
   <si>
-    <t>two wheller data</t>
-  </si>
-  <si>
     <t>warranty(quarter)</t>
+  </si>
+  <si>
+    <t>two wheller Data</t>
   </si>
 </sst>
 </file>
@@ -565,27 +565,27 @@
       </c>
       <c r="C7">
         <f ca="1">RANDBETWEEN(10,35)</f>
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D7">
         <f t="shared" ref="D7:H7" ca="1" si="0">RANDBETWEEN(10,35)</f>
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="L7" t="s">
         <v>1</v>
@@ -615,27 +615,27 @@
       </c>
       <c r="C8">
         <f ca="1">RANDBETWEEN(10000,40000)</f>
-        <v>14559</v>
+        <v>35455</v>
       </c>
       <c r="D8">
         <f t="shared" ref="D8:H8" ca="1" si="1">RANDBETWEEN(10000,40000)</f>
-        <v>35791</v>
+        <v>17006</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>16414</v>
+        <v>11012</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="1"/>
-        <v>36733</v>
+        <v>13015</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="1"/>
-        <v>12267</v>
+        <v>11592</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="1"/>
-        <v>20845</v>
+        <v>35821</v>
       </c>
       <c r="L8" t="s">
         <v>2</v>
@@ -673,15 +673,15 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="2"/>
@@ -715,27 +715,27 @@
       </c>
       <c r="C10">
         <f ca="1">($F$4/100)*C8</f>
-        <v>2911.8</v>
+        <v>7091</v>
       </c>
       <c r="D10">
         <f t="shared" ref="D10:H10" ca="1" si="3">($F$4/100)*D8</f>
-        <v>7158.2000000000007</v>
+        <v>3401.2000000000003</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="3"/>
-        <v>3282.8</v>
+        <v>2202.4</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="3"/>
-        <v>7346.6</v>
+        <v>2603</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="3"/>
-        <v>2453.4</v>
+        <v>2318.4</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="3"/>
-        <v>4169</v>
+        <v>7164.2000000000007</v>
       </c>
       <c r="L10" t="s">
         <v>5</v>
@@ -765,7 +765,7 @@
       </c>
       <c r="C11">
         <f ca="1">RANDBETWEEN(6,24)</f>
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D11">
         <f t="shared" ref="D11:H11" ca="1" si="4">RANDBETWEEN(6,24)</f>
@@ -773,19 +773,19 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="4"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="4"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="4"/>
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="L11" t="s">
         <v>4</v>
@@ -889,23 +889,23 @@
       </c>
       <c r="C7">
         <f ca="1">RANDBETWEEN(10,35)</f>
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D7">
         <f t="shared" ref="D7:G7" ca="1" si="0">RANDBETWEEN(10,35)</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="M7" t="s">
         <v>1</v>
@@ -932,23 +932,23 @@
       </c>
       <c r="C8">
         <f ca="1">RANDBETWEEN(5000,15000)</f>
-        <v>6664</v>
+        <v>7719</v>
       </c>
       <c r="D8">
         <f t="shared" ref="D8:G8" ca="1" si="1">RANDBETWEEN(5000,15000)</f>
-        <v>10740</v>
+        <v>14032</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>7875</v>
+        <v>14582</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="1"/>
-        <v>14820</v>
+        <v>7899</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="1"/>
-        <v>7194</v>
+        <v>12864</v>
       </c>
       <c r="M8" t="s">
         <v>22</v>
@@ -975,23 +975,23 @@
       </c>
       <c r="C9">
         <f ca="1">RANDBETWEEN(200,500)</f>
-        <v>242</v>
+        <v>214</v>
       </c>
       <c r="D9">
         <f t="shared" ref="D9:G9" ca="1" si="2">RANDBETWEEN(200,500)</f>
-        <v>413</v>
+        <v>457</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="2"/>
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="2"/>
-        <v>440</v>
+        <v>488</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="2"/>
-        <v>338</v>
+        <v>325</v>
       </c>
       <c r="M9" t="s">
         <v>3</v>
@@ -1018,15 +1018,15 @@
       </c>
       <c r="C10">
         <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10">
         <f t="shared" ref="D10:G10" ca="1" si="3">RANDBETWEEN(1,5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="3"/>
@@ -1034,7 +1034,7 @@
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M10" t="s">
         <v>21</v>
@@ -1061,23 +1061,23 @@
       </c>
       <c r="C11">
         <f ca="1">($G$4/100)*C8+C9</f>
-        <v>441.91999999999996</v>
+        <v>445.57</v>
       </c>
       <c r="D11">
         <f t="shared" ref="D11:G11" ca="1" si="4">($G$4/100)*D8+D9</f>
-        <v>735.2</v>
+        <v>877.96</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="4"/>
-        <v>526.25</v>
+        <v>718.46</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="4"/>
-        <v>884.59999999999991</v>
+        <v>724.97</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="4"/>
-        <v>553.81999999999994</v>
+        <v>710.92</v>
       </c>
       <c r="M11" t="s">
         <v>5</v>
@@ -1174,23 +1174,23 @@
       </c>
       <c r="D8">
         <f ca="1">RANDBETWEEN(6,36)</f>
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="E8">
         <f t="shared" ref="E8:H8" ca="1" si="0">RANDBETWEEN(6,36)</f>
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M8" t="s">
         <v>1</v>
@@ -1217,23 +1217,23 @@
       </c>
       <c r="D9">
         <f ca="1">RANDBETWEEN(445,1678)</f>
-        <v>717</v>
+        <v>453</v>
       </c>
       <c r="E9">
         <f t="shared" ref="E9:H9" ca="1" si="1">RANDBETWEEN(445,1678)</f>
-        <v>1500</v>
+        <v>1655</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="1"/>
-        <v>1326</v>
+        <v>1123</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="1"/>
-        <v>518</v>
+        <v>1616</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="1"/>
-        <v>1130</v>
+        <v>633</v>
       </c>
       <c r="M9" t="s">
         <v>30</v>
@@ -1260,23 +1260,23 @@
       </c>
       <c r="D10">
         <f ca="1">RANDBETWEEN(1234,6784)</f>
-        <v>6058</v>
+        <v>4751</v>
       </c>
       <c r="E10">
         <f t="shared" ref="E10:H10" ca="1" si="2">RANDBETWEEN(1234,6784)</f>
-        <v>5848</v>
+        <v>2552</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="2"/>
-        <v>2326</v>
+        <v>5981</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="2"/>
-        <v>4296</v>
+        <v>4899</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="2"/>
-        <v>1502</v>
+        <v>1787</v>
       </c>
       <c r="M10" t="s">
         <v>3</v>
@@ -1303,23 +1303,23 @@
       </c>
       <c r="D11">
         <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11">
         <f t="shared" ref="E11:H11" ca="1" si="3">RANDBETWEEN(1,5)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M11" t="s">
         <v>29</v>
@@ -1346,23 +1346,23 @@
       </c>
       <c r="D12">
         <f ca="1">($I$5/100)*D9</f>
-        <v>14.34</v>
+        <v>9.06</v>
       </c>
       <c r="E12">
         <f t="shared" ref="E12:H12" ca="1" si="4">($I$5/100)*E9</f>
-        <v>30</v>
+        <v>33.1</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="4"/>
-        <v>26.52</v>
+        <v>22.46</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="4"/>
-        <v>10.36</v>
+        <v>32.32</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="4"/>
-        <v>22.6</v>
+        <v>12.66</v>
       </c>
       <c r="M12" t="s">
         <v>5</v>
@@ -1461,23 +1461,23 @@
       </c>
       <c r="D9">
         <f ca="1">RANDBETWEEN(40,60)</f>
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E9">
         <f t="shared" ref="E9:H9" ca="1" si="0">RANDBETWEEN(40,60)</f>
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="3:18" x14ac:dyDescent="0.3">
@@ -1486,23 +1486,23 @@
       </c>
       <c r="D10">
         <f ca="1">RANDBETWEEN(10,30)</f>
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E10">
         <f t="shared" ref="E10:G10" ca="1" si="1">RANDBETWEEN(10,30)</f>
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="1"/>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H10">
         <f ca="1">RANDBETWEEN(10,30)</f>
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="3:18" x14ac:dyDescent="0.3">
@@ -1511,23 +1511,23 @@
       </c>
       <c r="D11">
         <f ca="1">RANDBETWEEN(30,100)</f>
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="E11">
         <f t="shared" ref="E11:H11" ca="1" si="2">RANDBETWEEN(30,100)</f>
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="2"/>
-        <v>82</v>
+        <v>38</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="2"/>
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="2"/>
-        <v>46</v>
+        <v>81</v>
       </c>
       <c r="M11" t="s">
         <v>1</v>
@@ -1554,23 +1554,23 @@
       </c>
       <c r="D12">
         <f ca="1">D10*D11</f>
-        <v>1647</v>
+        <v>1462</v>
       </c>
       <c r="E12">
         <f t="shared" ref="E12:H12" ca="1" si="3">E10*E11</f>
-        <v>1652</v>
+        <v>1100</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="3"/>
-        <v>1804</v>
+        <v>912</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="3"/>
-        <v>1360</v>
+        <v>836</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="3"/>
-        <v>1380</v>
+        <v>1458</v>
       </c>
       <c r="M12" t="s">
         <v>20</v>
@@ -1597,23 +1597,23 @@
       </c>
       <c r="D13">
         <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E13">
         <f t="shared" ref="E13:H13" ca="1" si="4">RANDBETWEEN(1,5)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M13" t="s">
         <v>37</v>
@@ -1640,23 +1640,23 @@
       </c>
       <c r="D14">
         <f ca="1">($H$6/100)*D12</f>
-        <v>98.82</v>
+        <v>87.72</v>
       </c>
       <c r="E14">
         <f t="shared" ref="E14:H14" ca="1" si="5">($H$6/100)*E12</f>
-        <v>99.11999999999999</v>
+        <v>66</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="5"/>
-        <v>108.24</v>
+        <v>54.72</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="5"/>
-        <v>81.599999999999994</v>
+        <v>50.16</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="5"/>
-        <v>82.8</v>
+        <v>87.47999999999999</v>
       </c>
       <c r="M14" t="s">
         <v>38</v>
@@ -1792,23 +1792,23 @@
       </c>
       <c r="D7">
         <f ca="1">RANDBETWEEN(20,50)</f>
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="E7">
         <f t="shared" ref="E7:H7" ca="1" si="0">RANDBETWEEN(20,50)</f>
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="3:18" x14ac:dyDescent="0.3">
@@ -1817,23 +1817,23 @@
       </c>
       <c r="D8">
         <f ca="1">RANDBETWEEN(200,500)</f>
-        <v>328</v>
+        <v>440</v>
       </c>
       <c r="E8">
         <f t="shared" ref="E8:H8" ca="1" si="1">RANDBETWEEN(200,500)</f>
-        <v>290</v>
+        <v>388</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="1"/>
-        <v>462</v>
+        <v>480</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="1"/>
-        <v>416</v>
+        <v>328</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="1"/>
-        <v>451</v>
+        <v>498</v>
       </c>
     </row>
     <row r="9" spans="3:18" x14ac:dyDescent="0.3">
@@ -1842,15 +1842,15 @@
       </c>
       <c r="D9">
         <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9">
         <f t="shared" ref="E9:H9" ca="1" si="2">RANDBETWEEN(1,5)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="2"/>
@@ -1858,7 +1858,7 @@
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="3:18" x14ac:dyDescent="0.3">
@@ -1867,23 +1867,23 @@
       </c>
       <c r="D10">
         <f ca="1">RANDBETWEEN(134765,856342)</f>
-        <v>663769</v>
+        <v>378071</v>
       </c>
       <c r="E10">
         <f t="shared" ref="E10:H10" ca="1" si="3">RANDBETWEEN(134765,856342)</f>
-        <v>383316</v>
+        <v>305469</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="3"/>
-        <v>385295</v>
+        <v>569154</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="3"/>
-        <v>603600</v>
+        <v>485892</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="3"/>
-        <v>506242</v>
+        <v>403143</v>
       </c>
     </row>
     <row r="11" spans="3:18" x14ac:dyDescent="0.3">
@@ -1892,23 +1892,23 @@
       </c>
       <c r="D11">
         <f ca="1">($I$4/100)*D8</f>
-        <v>4.92</v>
+        <v>6.6</v>
       </c>
       <c r="E11">
         <f t="shared" ref="E11:H11" ca="1" si="4">($I$4/100)*E8</f>
-        <v>4.3499999999999996</v>
+        <v>5.8199999999999994</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="4"/>
-        <v>6.93</v>
+        <v>7.1999999999999993</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="4"/>
-        <v>6.24</v>
+        <v>4.92</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="4"/>
-        <v>6.7649999999999997</v>
+        <v>7.47</v>
       </c>
     </row>
     <row r="12" spans="3:18" x14ac:dyDescent="0.3">
@@ -2041,7 +2041,7 @@
   <dimension ref="C5:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2054,7 +2054,7 @@
   <sheetData>
     <row r="5" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G5" t="s">
         <v>4</v>
@@ -2089,23 +2089,23 @@
       </c>
       <c r="D9">
         <f ca="1">RANDBETWEEN(5,15)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9">
         <f t="shared" ref="E9:H9" ca="1" si="0">RANDBETWEEN(5,15)</f>
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="3:18" x14ac:dyDescent="0.3">
@@ -2114,44 +2114,44 @@
       </c>
       <c r="D10">
         <f ca="1">RANDBETWEEN(50000,100000)</f>
-        <v>52304</v>
+        <v>75783</v>
       </c>
       <c r="E10">
         <f t="shared" ref="E10:H10" ca="1" si="1">RANDBETWEEN(50000,100000)</f>
-        <v>52157</v>
+        <v>65201</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="1"/>
-        <v>98327</v>
+        <v>89073</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="1"/>
-        <v>61519</v>
+        <v>64903</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="1"/>
-        <v>81765</v>
+        <v>93099</v>
       </c>
     </row>
     <row r="11" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11">
         <f ca="1">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E11">
         <f t="shared" ref="E11:H11" ca="1" si="2">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="2"/>
@@ -2168,7 +2168,7 @@
       </c>
       <c r="E12">
         <f t="shared" ref="E12:H12" ca="1" si="3">RANDBETWEEN(1,5)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="3"/>
@@ -2176,11 +2176,11 @@
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="3:18" x14ac:dyDescent="0.3">
@@ -2189,23 +2189,23 @@
       </c>
       <c r="D13">
         <f ca="1">($H$5/100)*D10</f>
-        <v>6276.48</v>
+        <v>9093.9599999999991</v>
       </c>
       <c r="E13">
         <f t="shared" ref="E13:H13" ca="1" si="4">($H$5/100)*E10</f>
-        <v>6258.84</v>
+        <v>7824.12</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="4"/>
-        <v>11799.24</v>
+        <v>10688.76</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="4"/>
-        <v>7382.28</v>
+        <v>7788.36</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="4"/>
-        <v>9811.7999999999993</v>
+        <v>11171.88</v>
       </c>
       <c r="M13" t="s">
         <v>1</v>
@@ -2268,7 +2268,7 @@
     </row>
     <row r="16" spans="3:18" x14ac:dyDescent="0.3">
       <c r="M16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N16">
         <v>1</v>

</xml_diff>